<commit_message>
label match feature done
</commit_message>
<xml_diff>
--- a/Liushui/nn/xlsx_files/system type rules.xlsx
+++ b/Liushui/nn/xlsx_files/system type rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentl/PycharmProjects/Aita-Tech/Liushui/nn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentl/PycharmProjects/Aita-Tech/Liushui/nn/xlsx_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CAEFD6-80AB-E34D-B157-A5928E23DE0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A07A43-ED9D-8042-B328-A2B1A5E6D2ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32240" yWindow="6880" windowWidth="27920" windowHeight="20540" activeTab="1" xr2:uid="{B0706080-C193-46F5-88CF-D3F562155D47}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">现金流量表!$A$2:$C$50</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="129">
   <si>
     <r>
       <rPr>
@@ -784,6 +784,10 @@
   </si>
   <si>
     <t>废品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>投资收益</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1879,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF4615D-20C3-4AD3-8168-4660B6CCB643}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="141" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2159,7 +2163,7 @@
       <c r="A27" s="23"/>
       <c r="B27" s="22"/>
       <c r="C27" s="11" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>72</v>

</xml_diff>